<commit_message>
docs and vars print
</commit_message>
<xml_diff>
--- a/bi/docs/resultsTable.xlsx
+++ b/bi/docs/resultsTable.xlsx
@@ -3,14 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20325"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7918E509-9E42-4CC8-9520-CBC01C17A19E}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02521CEA-E788-45CD-A968-D21C6F4681F9}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="179021"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -446,7 +446,7 @@
   <dimension ref="A1:H22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -717,12 +717,22 @@
       <c r="A12" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B12" s="2"/>
+      <c r="B12" s="2">
+        <v>54.152000000000001</v>
+      </c>
       <c r="C12" s="4"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-      <c r="G12" s="2"/>
+      <c r="D12" s="2">
+        <v>54.152000000000001</v>
+      </c>
+      <c r="E12" s="2">
+        <v>20</v>
+      </c>
+      <c r="F12" s="2">
+        <v>200</v>
+      </c>
+      <c r="G12" s="2">
+        <v>300</v>
+      </c>
       <c r="H12" s="1"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -821,9 +831,15 @@
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
-      <c r="B22" s="2"/>
+      <c r="B22" s="2">
+        <f>MAX(B5:B21)</f>
+        <v>54.51</v>
+      </c>
       <c r="C22" s="4"/>
-      <c r="D22" s="2"/>
+      <c r="D22" s="2">
+        <f>MAX(D5:D21)</f>
+        <v>54.152000000000001</v>
+      </c>
       <c r="E22" s="2"/>
       <c r="F22" s="2"/>
       <c r="G22" s="2"/>

</xml_diff>

<commit_message>
multi rnn and xavier init
</commit_message>
<xml_diff>
--- a/bi/docs/resultsTable.xlsx
+++ b/bi/docs/resultsTable.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20325"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D262E089-4AE7-4C33-8765-7D099227FA4D}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32ACB9C8-7F8E-4C32-88D1-2F4CDB2FDF30}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="42">
   <si>
     <t>train acc</t>
   </si>
@@ -143,6 +143,9 @@
   </si>
   <si>
     <t>17. 5 way 300dim</t>
+  </si>
+  <si>
+    <t>5/10</t>
   </si>
 </sst>
 </file>
@@ -497,7 +500,7 @@
   <dimension ref="A1:I22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1003,8 +1006,12 @@
       <c r="A19" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B19" s="2"/>
-      <c r="C19" s="4"/>
+      <c r="B19" s="2">
+        <v>56.14</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>41</v>
+      </c>
       <c r="D19" s="2"/>
       <c r="E19" s="2">
         <v>10</v>
@@ -1026,8 +1033,12 @@
       <c r="A20" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B20" s="2"/>
-      <c r="C20" s="4"/>
+      <c r="B20" s="2">
+        <v>54.46</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>19</v>
+      </c>
       <c r="D20" s="2"/>
       <c r="E20" s="2">
         <v>20</v>

</xml_diff>